<commit_message>
updated cart validation -1 web and db
</commit_message>
<xml_diff>
--- a/InputFiles/TC47_Canine_Filter_Breed-YorkshireTerr.xlsx
+++ b/InputFiles/TC47_Canine_Filter_Breed-YorkshireTerr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A88070-07FA-4953-AF6F-469FD69402B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1BE972-D866-4CF2-AD94-A913703B8028}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -132,6 +132,36 @@
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+  </si>
+  <si>
+    <t>cartQuery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+  WHERE demo.breed IN ['Yorkshire Terrier']
+MATCH (f:file)-[*]-&gt;(c)
+WITH COLLECT(DISTINCT f.uuid) AS uuids
+MATCH (f:file)
+  WHERE f.uuid in uuids
+OPTIONAL MATCH (f)--&gt;(parent)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c:case)
+OPTIONAL MATCH (s:study)&lt;-[:member_of]-(c)
+OPTIONAL MATCH (c)--&gt;(i:canine_individual)&lt;--(o:case)
+RETURN
+  f.file_name AS `File Name`,
+  f.file_type AS `File Type`,
+  head(labels(parent)) AS `Association`,
+  f.file_description AS `Description`,
+  f.file_format AS `Format`,
+  f.file_size AS `Size`,
+  samp.sample_id AS `Sample ID`,
+  c.case_id as `Case ID`,
+  i.canine_individual_id AS `Canine ID`,
+  CASE WHEN s.clinical_study_designation IS NULL 
+  THEN parent.clinical_study_designation 
+  ELSE s.clinical_study_designation END AS `Study Code`
+  </t>
   </si>
 </sst>
 </file>
@@ -501,22 +531,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.44140625" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" customWidth="1"/>
+    <col min="3" max="4" width="75.7109375" customWidth="1"/>
+    <col min="5" max="5" width="70.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -527,13 +557,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -543,14 +576,17 @@
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -560,14 +596,17 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -577,10 +616,13 @@
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>